<commit_message>
Changed data in excel file
</commit_message>
<xml_diff>
--- a/src/test/java/com/internetBanking/testData/LoginData.xlsx
+++ b/src/test/java/com/internetBanking/testData/LoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7AC43FE-DA2F-4E14-9241-4DA9A76D3A69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DA570A-77CA-4792-A3E8-722F535E5E8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53145" yWindow="2835" windowWidth="16875" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>mngr83460</t>
-  </si>
-  <si>
-    <t>qAbUzyj</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -34,29 +28,20 @@
     <t>password</t>
   </si>
   <si>
-    <t>mngr112909</t>
+    <t>mEmYsUj</t>
   </si>
   <si>
-    <t>tytUreg</t>
+    <t>mngr258526</t>
   </si>
   <si>
-    <t>mngr164225</t>
-  </si>
-  <si>
-    <t>jahetAp</t>
-  </si>
-  <si>
-    <t>mngr258528</t>
-  </si>
-  <si>
-    <t>mEmYsUj</t>
+    <t>mngr258527</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +60,12 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -442,7 +433,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -453,53 +444,42 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>